<commit_message>
Cambios en el archivo excel de Reporte Eventos
</commit_message>
<xml_diff>
--- a/assets/Registro_Eventos_Discoteca.xlsx
+++ b/assets/Registro_Eventos_Discoteca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7276906cda80b93/Escritorio/informeCatrinaMagika2024/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54B4E3C6-72D7-460B-A5F2-0B75CDF39FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{54B4E3C6-72D7-460B-A5F2-0B75CDF39FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC113393-925C-4648-ABAE-180035DC5AF5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>14 de Diciembre de 2024</t>
+  </si>
+  <si>
+    <t>Asumidos por el Organizador</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -397,89 +400,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,7 +516,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>933449</xdr:rowOff>
     </xdr:to>
@@ -555,7 +557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="8410575" cy="2076449"/>
+          <a:ext cx="8801100" cy="2076449"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -856,15 +858,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
@@ -872,781 +874,700 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="3">
         <v>21896000</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="29"/>
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="3">
         <v>12024963</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="3">
         <v>9871037</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="9" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12">
+      <c r="C15" s="23"/>
+      <c r="D15" s="24">
         <v>2934677</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12">
+      <c r="C16" s="23"/>
+      <c r="D16" s="24">
         <v>5638000</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12">
+      <c r="C17" s="23"/>
+      <c r="D17" s="24">
         <v>2300000</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12">
+      <c r="C18" s="23"/>
+      <c r="D18" s="24">
         <v>100000</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12">
+      <c r="C19" s="23"/>
+      <c r="D19" s="24">
         <v>490780</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="11" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12">
+      <c r="C20" s="23"/>
+      <c r="D20" s="24">
         <v>120000</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="1"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="11" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12">
+      <c r="C21" s="23"/>
+      <c r="D21" s="24">
         <v>441506</v>
       </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="1"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="17"/>
+      <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="1"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="17"/>
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="3" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="3">
         <v>9000000</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="3">
         <v>3364650</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="3">
         <v>5635350</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="17"/>
+      <c r="B28" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="1"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="17"/>
     </row>
     <row r="29" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="9" t="s">
+      <c r="C29" s="22"/>
+      <c r="D29" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="11" t="s">
+      <c r="E29" s="22"/>
+      <c r="F29" s="17"/>
+    </row>
+    <row r="30" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12">
-        <v>2934677</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="19" t="s">
+      <c r="C30" s="23"/>
+      <c r="D30" s="24">
+        <v>1064650</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20">
-        <v>1800000</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22">
-        <v>100000</v>
-      </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="1"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26">
+        <v>2100000</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11">
+        <v>200000</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="17"/>
     </row>
     <row r="33" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="17"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="17"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="17"/>
+    </row>
+    <row r="35" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="17"/>
+    </row>
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="17"/>
+    </row>
+    <row r="37" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3">
+        <v>23946370</v>
+      </c>
+      <c r="F37" s="17"/>
+    </row>
+    <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="3">
+        <v>8612367</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="3">
+        <v>15334003</v>
+      </c>
+      <c r="F38" s="17"/>
+    </row>
+    <row r="39" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="22"/>
+      <c r="F40" s="17"/>
+    </row>
+    <row r="41" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24">
+        <v>1366997</v>
+      </c>
+      <c r="E41" s="24"/>
+      <c r="F41" s="17"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="26">
+        <v>450000</v>
+      </c>
+      <c r="E42" s="26"/>
+      <c r="F42" s="17"/>
+    </row>
+    <row r="43" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3" t="s">
+      <c r="C43" s="10"/>
+      <c r="D43" s="11">
+        <v>182919</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="17"/>
+    </row>
+    <row r="44" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="17"/>
+      <c r="B44" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11">
+        <v>440000</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11">
+        <v>1890000</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="17"/>
+    </row>
+    <row r="46" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11">
+        <v>232500</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="F46" s="17"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11">
+        <v>57000</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="17"/>
+    </row>
+    <row r="48" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="17"/>
+      <c r="B48" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11">
+        <v>183000</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="17"/>
+    </row>
+    <row r="49" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="17"/>
+      <c r="B49" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="11">
+        <v>3810000</v>
+      </c>
+      <c r="E49" s="11"/>
+      <c r="F49" s="17"/>
+    </row>
+    <row r="50" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="17"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="17"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="17"/>
+    </row>
+    <row r="52" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="17"/>
+      <c r="B52" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3" t="s">
+      <c r="C52" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="13"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="17"/>
+    </row>
+    <row r="53" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="17"/>
+      <c r="B53" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C53" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="3" t="s">
+      <c r="E53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" s="17"/>
+    </row>
+    <row r="54" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="17"/>
+      <c r="B54" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="3" t="s">
+      <c r="C54" s="7"/>
+      <c r="D54" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E38" s="8">
-        <v>23946370</v>
-      </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="3" t="s">
+      <c r="E54" s="6">
+        <v>5000000</v>
+      </c>
+      <c r="F54" s="17"/>
+    </row>
+    <row r="55" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="17"/>
+      <c r="B55" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="8">
-        <v>8612367</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="C55" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="8">
-        <v>15334003</v>
-      </c>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12">
-        <v>1366997</v>
-      </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20">
-        <v>450000</v>
-      </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="22">
-        <v>182919</v>
-      </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="21"/>
-      <c r="D45" s="22">
-        <v>440000</v>
-      </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="21"/>
-      <c r="D46" s="22">
-        <v>1890000</v>
-      </c>
-      <c r="E46" s="22"/>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="22">
-        <v>232500</v>
-      </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="22">
-        <v>57000</v>
-      </c>
-      <c r="E48" s="22"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="22">
-        <v>183000</v>
-      </c>
-      <c r="E49" s="22"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="22">
-        <v>3810000</v>
-      </c>
-      <c r="E50" s="22"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D53" s="17"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" s="24">
+      <c r="E55" s="9">
         <v>5000000</v>
       </c>
-      <c r="F55" s="1"/>
+      <c r="F55" s="17"/>
     </row>
     <row r="56" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" s="27">
-        <v>5000000</v>
-      </c>
-      <c r="F56" s="1"/>
+      <c r="A56" s="17"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="17"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="1"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="A58" s="17"/>
+      <c r="F58" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="B51:E52"/>
-    <mergeCell ref="B57:E58"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="A22:F23"/>
-    <mergeCell ref="A24:A58"/>
-    <mergeCell ref="F24:F58"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:E35"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
+  <mergeCells count="61">
+    <mergeCell ref="F8:F21"/>
     <mergeCell ref="A1:E7"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A9:A21"/>
@@ -1663,7 +1584,50 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F8:F21"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="A22:F23"/>
+    <mergeCell ref="A24:A58"/>
+    <mergeCell ref="F24:F58"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B33:E34"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="B50:E51"/>
+    <mergeCell ref="B56:E57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio en el archivo resumen de eventos 2024
</commit_message>
<xml_diff>
--- a/assets/Registro_Eventos_Discoteca.xlsx
+++ b/assets/Registro_Eventos_Discoteca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7276906cda80b93/Escritorio/informeCatrinaMagika2024/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{54B4E3C6-72D7-460B-A5F2-0B75CDF39FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC113393-925C-4648-ABAE-180035DC5AF5}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{54B4E3C6-72D7-460B-A5F2-0B75CDF39FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ACF5764-8023-498A-8AD5-6A036E410C6D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,61 +427,61 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,6 +567,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -858,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56:E57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,13 +878,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -888,11 +892,11 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -900,11 +904,11 @@
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -912,11 +916,11 @@
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -924,11 +928,11 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -936,11 +940,11 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -948,11 +952,11 @@
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -960,27 +964,27 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="17"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="17"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
@@ -993,10 +997,10 @@
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="17"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1009,10 +1013,10 @@
       <c r="E11" s="3">
         <v>21896000</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1025,144 +1029,144 @@
       <c r="E12" s="3">
         <v>9871037</v>
       </c>
-      <c r="F12" s="17"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="17"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="21" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24">
+      <c r="C15" s="14"/>
+      <c r="D15" s="15">
         <v>2934677</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="17"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="23" t="s">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24">
+      <c r="C16" s="14"/>
+      <c r="D16" s="15">
         <v>5638000</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="17"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="23" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24">
+      <c r="C17" s="14"/>
+      <c r="D17" s="15">
         <v>2300000</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="17"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="23" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24">
+      <c r="C18" s="14"/>
+      <c r="D18" s="15">
         <v>100000</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="17"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="23" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24">
+      <c r="C19" s="14"/>
+      <c r="D19" s="15">
         <v>490780</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="17"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="24">
+      <c r="C20" s="14"/>
+      <c r="D20" s="15">
         <v>120000</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="17"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="23" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24">
+      <c r="C21" s="14"/>
+      <c r="D21" s="15">
         <v>441506</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="17"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="17"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1175,10 +1179,10 @@
       <c r="E25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="17"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1189,10 +1193,10 @@
       <c r="E26" s="3">
         <v>9000000</v>
       </c>
-      <c r="F26" s="17"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1205,96 +1209,96 @@
       <c r="E27" s="3">
         <v>5635350</v>
       </c>
-      <c r="F27" s="17"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="17"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="10"/>
+      <c r="B29" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="21" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="23" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15">
         <v>1064650</v>
       </c>
-      <c r="E30" s="24"/>
-      <c r="F30" s="17"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="25" t="s">
+      <c r="A31" s="10"/>
+      <c r="B31" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26">
+      <c r="C31" s="21"/>
+      <c r="D31" s="22">
         <v>2100000</v>
       </c>
-      <c r="E31" s="26"/>
-      <c r="F31" s="17"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="10"/>
+      <c r="B32" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11">
+      <c r="C32" s="26"/>
+      <c r="D32" s="27">
         <v>200000</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="17"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="17"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="17"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="17"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="1" t="s">
         <v>2</v>
       </c>
@@ -1307,10 +1311,10 @@
       <c r="E36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="17"/>
+      <c r="F36" s="10"/>
     </row>
     <row r="37" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
@@ -1323,10 +1327,10 @@
       <c r="E37" s="3">
         <v>23946370</v>
       </c>
-      <c r="F37" s="17"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1339,168 +1343,168 @@
       <c r="E38" s="3">
         <v>15334003</v>
       </c>
-      <c r="F38" s="17"/>
+      <c r="F38" s="10"/>
     </row>
     <row r="39" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
       <c r="E39" s="20"/>
-      <c r="F39" s="17"/>
+      <c r="F39" s="10"/>
     </row>
     <row r="40" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="21" t="s">
+      <c r="A40" s="10"/>
+      <c r="B40" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="21" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="22"/>
-      <c r="F40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="23" t="s">
+      <c r="A41" s="10"/>
+      <c r="B41" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="24">
+      <c r="C41" s="14"/>
+      <c r="D41" s="15">
         <v>1366997</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="17"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
-      <c r="B42" s="25" t="s">
+      <c r="A42" s="10"/>
+      <c r="B42" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="26">
+      <c r="C42" s="21"/>
+      <c r="D42" s="22">
         <v>450000</v>
       </c>
-      <c r="E42" s="26"/>
-      <c r="F42" s="17"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="10"/>
     </row>
     <row r="43" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="10" t="s">
+      <c r="A43" s="10"/>
+      <c r="B43" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="11">
+      <c r="C43" s="26"/>
+      <c r="D43" s="27">
         <v>182919</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="17"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="10" t="s">
+      <c r="A44" s="10"/>
+      <c r="B44" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11">
+      <c r="C44" s="26"/>
+      <c r="D44" s="27">
         <v>440000</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="17"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="10" t="s">
+      <c r="A45" s="10"/>
+      <c r="B45" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11">
+      <c r="C45" s="26"/>
+      <c r="D45" s="27">
         <v>1890000</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="17"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="10" t="s">
+      <c r="A46" s="10"/>
+      <c r="B46" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11">
+      <c r="C46" s="26"/>
+      <c r="D46" s="27">
         <v>232500</v>
       </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="17"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="10"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="17"/>
-      <c r="B47" s="10" t="s">
+      <c r="A47" s="10"/>
+      <c r="B47" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="11">
+      <c r="C47" s="26"/>
+      <c r="D47" s="27">
         <v>57000</v>
       </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="17"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="10"/>
     </row>
     <row r="48" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17"/>
-      <c r="B48" s="10" t="s">
+      <c r="A48" s="10"/>
+      <c r="B48" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="11">
+      <c r="C48" s="26"/>
+      <c r="D48" s="27">
         <v>183000</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="17"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="10"/>
     </row>
     <row r="49" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="10" t="s">
+      <c r="A49" s="10"/>
+      <c r="B49" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="11">
+      <c r="C49" s="26"/>
+      <c r="D49" s="27">
         <v>3810000</v>
       </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="17"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="10"/>
     </row>
     <row r="50" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="17"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="17"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="10"/>
     </row>
     <row r="52" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D52" s="13"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="17"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="10"/>
     </row>
     <row r="53" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="1" t="s">
         <v>2</v>
       </c>
@@ -1513,10 +1517,10 @@
       <c r="E53" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F53" s="17"/>
+      <c r="F53" s="10"/>
     </row>
     <row r="54" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="5" t="s">
         <v>5</v>
       </c>
@@ -1527,10 +1531,10 @@
       <c r="E54" s="6">
         <v>5000000</v>
       </c>
-      <c r="F54" s="17"/>
+      <c r="F54" s="10"/>
     </row>
     <row r="55" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="8" t="s">
         <v>9</v>
       </c>
@@ -1543,30 +1547,75 @@
       <c r="E55" s="9">
         <v>5000000</v>
       </c>
-      <c r="F55" s="17"/>
+      <c r="F55" s="10"/>
     </row>
     <row r="56" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="17"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="10"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="F58" s="17"/>
+      <c r="A58" s="10"/>
+      <c r="F58" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="B50:E51"/>
+    <mergeCell ref="B56:E57"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="A22:F23"/>
+    <mergeCell ref="A24:A58"/>
+    <mergeCell ref="F24:F58"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B33:E34"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="F8:F21"/>
     <mergeCell ref="A1:E7"/>
     <mergeCell ref="A8:E8"/>
@@ -1583,51 +1632,6 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="A22:F23"/>
-    <mergeCell ref="A24:A58"/>
-    <mergeCell ref="F24:F58"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:E34"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="B50:E51"/>
-    <mergeCell ref="B56:E57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>